<commit_message>
Add XLOOKUP tutorial file and update formula template in Excel
</commit_message>
<xml_diff>
--- a/Excel/Formula Excel Template.xlsx
+++ b/Excel/Formula Excel Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\sql_practice\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5732435-2380-45E3-82CC-01896F7ACDAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F3DFB7-06DA-4B83-A82D-5985D5CAC8FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15487" yWindow="0" windowWidth="10193" windowHeight="14480" firstSheet="5" activeTab="6" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
+    <workbookView xWindow="15487" yWindow="0" windowWidth="10193" windowHeight="14480" firstSheet="10" activeTab="10" xr2:uid="{47981922-77C5-4EC3-A76E-98D6CE997DC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Max-Min" sheetId="9" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="91">
   <si>
     <t>FirstName</t>
   </si>
@@ -330,6 +330,15 @@
   </si>
   <si>
     <t>right</t>
+  </si>
+  <si>
+    <t>04/17/1996</t>
+  </si>
+  <si>
+    <t>03/26/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1352,14 +1361,15 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
+    <col min="6" max="6" width="15.76171875" customWidth="1"/>
     <col min="8" max="8" width="14.41015625" customWidth="1"/>
     <col min="9" max="9" width="13.3515625" customWidth="1"/>
   </cols>
@@ -1427,6 +1437,14 @@
       <c r="I2" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="J2">
+        <f>_xlfn.DAYS(I2,H2)</f>
+        <v>5056</v>
+      </c>
+      <c r="K2">
+        <f>NETWORKDAYS(H2,I2)</f>
+        <v>3611</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3">
@@ -1456,6 +1474,10 @@
       <c r="I3" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J10" si="0">_xlfn.DAYS(I3,H3)</f>
+        <v>5851</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4">
@@ -1485,6 +1507,10 @@
       <c r="I4" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>6275</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5">
@@ -1514,6 +1540,10 @@
       <c r="I5" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>5811</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6">
@@ -1543,6 +1573,10 @@
       <c r="I6" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>5960</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7">
@@ -1572,6 +1606,10 @@
       <c r="I7" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>4511</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8">
@@ -1601,6 +1639,10 @@
       <c r="I8" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>3595</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9">
@@ -1630,6 +1672,10 @@
       <c r="I9" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>4700</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10">
@@ -1654,10 +1700,19 @@
         <v>42000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>61</v>
+        <v>89</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>10570</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.5">
+      <c r="H18" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -3506,7 +3561,7 @@
   </sheetPr>
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L10"/>
     </sheetView>
   </sheetViews>
@@ -3972,8 +4027,8 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4043,6 +4098,18 @@
       </c>
       <c r="I2" s="1">
         <v>42253</v>
+      </c>
+      <c r="J2">
+        <f>SUM(G2:G10)</f>
+        <v>437000</v>
+      </c>
+      <c r="K2">
+        <f>SUMIF(G2:G10, "&gt;35000")</f>
+        <v>437000</v>
+      </c>
+      <c r="L2">
+        <f>SUMIFS(G2:G10,E2:E10,"female",D2:D10,"&lt;32")</f>
+        <v>83000</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.5">
@@ -4289,8 +4356,8 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.64453125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4365,6 +4432,18 @@
       <c r="I2" s="1">
         <v>42253</v>
       </c>
+      <c r="J2">
+        <f>COUNT(G2:G10)</f>
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF(G2:G10,"&gt;50000")</f>
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <f>COUNTIFS(G2:G10,"&gt;50000",E2:E10,"Male")</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3">

</xml_diff>